<commit_message>
send & list mail in lecturer users
</commit_message>
<xml_diff>
--- a/student/upload/uploads/33826-new-microsoft-excel-worksheet.xlsx
+++ b/student/upload/uploads/33826-new-microsoft-excel-worksheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -144,6 +144,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +196,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +365,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>